<commit_message>
cleaning data folder from unused excel templates
</commit_message>
<xml_diff>
--- a/data/car_monitoring.xlsx
+++ b/data/car_monitoring.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSAran\Desktop\Files\duty\Uniss\EnhanceFAIRness_spreadsheet_to_db\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A621C98D-36CB-4679-AE47-0DB0727F9452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969E7C29-1D7F-4EDD-92C0-D6D2E2CBB156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{509A64F3-1995-4482-BAB9-2B4BA9D06CEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{509A64F3-1995-4482-BAB9-2B4BA9D06CEE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Brand" sheetId="1" r:id="rId1"/>
-    <sheet name="model" sheetId="4" r:id="rId2"/>
-    <sheet name="City" sheetId="2" r:id="rId3"/>
-    <sheet name="Users" sheetId="3" r:id="rId4"/>
-    <sheet name="DDict_Table" sheetId="18" r:id="rId5"/>
+    <sheet name="brand" sheetId="1" r:id="rId1"/>
+    <sheet name="car" sheetId="4" r:id="rId2"/>
+    <sheet name="model" sheetId="23" r:id="rId3"/>
+    <sheet name="city" sheetId="2" r:id="rId4"/>
+    <sheet name="employee" sheetId="3" r:id="rId5"/>
+    <sheet name="tables_infos" sheetId="28" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,14 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
-  <si>
-    <t>Brand_id</t>
-  </si>
-  <si>
-    <t>Brand_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>Alfa romeo</t>
   </si>
@@ -57,15 +74,6 @@
     <t>Fiat</t>
   </si>
   <si>
-    <t>Creation_date</t>
-  </si>
-  <si>
-    <t>City_id</t>
-  </si>
-  <si>
-    <t>City_name</t>
-  </si>
-  <si>
     <t>Turin</t>
   </si>
   <si>
@@ -99,9 +107,6 @@
     <t>user_id</t>
   </si>
   <si>
-    <t>authorized_user</t>
-  </si>
-  <si>
     <t>fiesta</t>
   </si>
   <si>
@@ -156,23 +161,68 @@
     <t>ReferenceTable</t>
   </si>
   <si>
-    <t>Brand</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Users</t>
+    <t>license_tag</t>
+  </si>
+  <si>
+    <t>GE-324-GV</t>
+  </si>
+  <si>
+    <t>RV-724-BL</t>
+  </si>
+  <si>
+    <t>AC-493-GH</t>
+  </si>
+  <si>
+    <t>BK-815-KL</t>
+  </si>
+  <si>
+    <t>PM-672-JN</t>
+  </si>
+  <si>
+    <t>MO-719-DS</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>brand_name</t>
+  </si>
+  <si>
+    <t>creation_date</t>
+  </si>
+  <si>
+    <t>city_id</t>
+  </si>
+  <si>
+    <t>city_name</t>
+  </si>
+  <si>
+    <t>car_id</t>
+  </si>
+  <si>
+    <t>img</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,16 +230,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -197,18 +267,210 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -225,53 +487,129 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BC3FE163-C03D-4703-B24C-7663328E7824}" name="Tableau1" displayName="Tableau1" ref="A1:D4" totalsRowShown="0">
   <autoFilter ref="A1:D4" xr:uid="{BC3FE163-C03D-4703-B24C-7663328E7824}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E4EFA1BA-A779-4B2B-83F3-94D09A056040}" name="Brand_id"/>
-    <tableColumn id="2" xr3:uid="{C8C549C4-0860-4BCE-9382-F247708BA5C3}" name="Brand_name"/>
-    <tableColumn id="3" xr3:uid="{614FD2B6-F108-42C6-AC15-A899556EE9A3}" name="Creation_date"/>
-    <tableColumn id="4" xr3:uid="{F619F83C-F0E0-4372-9DF1-5657EDEEF54A}" name="City_id"/>
+    <tableColumn id="1" xr3:uid="{E4EFA1BA-A779-4B2B-83F3-94D09A056040}" name="brand_id"/>
+    <tableColumn id="2" xr3:uid="{C8C549C4-0860-4BCE-9382-F247708BA5C3}" name="brand_name"/>
+    <tableColumn id="3" xr3:uid="{614FD2B6-F108-42C6-AC15-A899556EE9A3}" name="creation_date"/>
+    <tableColumn id="4" xr3:uid="{F619F83C-F0E0-4372-9DF1-5657EDEEF54A}" name="city_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6CF7D205-5C4D-4E92-BBE1-492D295F37FB}" name="Tableau2" displayName="Tableau2" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{6CF7D205-5C4D-4E92-BBE1-492D295F37FB}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AE78F5E7-0F4A-434D-A809-C6B6C10F763C}" name="model_id"/>
-    <tableColumn id="2" xr3:uid="{23F30DB4-9086-4625-B5A7-DF6B0BA2CA19}" name="brand_id"/>
-    <tableColumn id="3" xr3:uid="{45A6E397-D70A-4C15-955E-D77121AD97A7}" name="model_name"/>
-    <tableColumn id="4" xr3:uid="{F01B20AB-3B18-447F-807B-978676924EF4}" name="purchase date" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6CF7D205-5C4D-4E92-BBE1-492D295F37FB}" name="Tableau2" displayName="Tableau2" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{6CF7D205-5C4D-4E92-BBE1-492D295F37FB}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{AE78F5E7-0F4A-434D-A809-C6B6C10F763C}" name="license_tag"/>
+    <tableColumn id="2" xr3:uid="{23F30DB4-9086-4625-B5A7-DF6B0BA2CA19}" name="model_id"/>
+    <tableColumn id="4" xr3:uid="{F01B20AB-3B18-447F-807B-978676924EF4}" name="purchase date" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{1604D12D-73D0-4EAC-8182-B7C2923344E7}" name="kilometers"/>
-    <tableColumn id="6" xr3:uid="{7BC91CF3-A031-450C-A838-0D64030C8EB9}" name="authorized_user"/>
+    <tableColumn id="3" xr3:uid="{9B001820-4CA8-4D94-B634-6547A8030266}" name="img"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CCF7B60D-89B0-4270-B4D2-EF64FCAD8B03}" name="Tableau5" displayName="Tableau5" ref="A1:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C7" xr:uid="{CCF7B60D-89B0-4270-B4D2-EF64FCAD8B03}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9E6AF7E4-A8D5-4EB6-87C9-C4F64F4CFB07}" name="model_id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C195E5BC-013D-423A-9562-63FDF98EC6FE}" name="brand_id" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{951D8135-BD0E-41D6-8C77-15FA9147BE1E}" name="model_name" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6328ECB0-DB75-405B-8A2B-B3BFA256B2B5}" name="Tableau3" displayName="Tableau3" ref="A1:B3" totalsRowShown="0">
   <autoFilter ref="A1:B3" xr:uid="{6328ECB0-DB75-405B-8A2B-B3BFA256B2B5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6A1A739F-1F2D-4B19-BD97-861F2E5CB7D5}" name="City_id"/>
-    <tableColumn id="2" xr3:uid="{9F56575F-77B5-4BB7-B911-C689AE4BE3C2}" name="City_name"/>
+    <tableColumn id="1" xr3:uid="{6A1A739F-1F2D-4B19-BD97-861F2E5CB7D5}" name="city_id"/>
+    <tableColumn id="2" xr3:uid="{9F56575F-77B5-4BB7-B911-C689AE4BE3C2}" name="city_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{83DE1AE3-FEA1-4540-8E88-7AF1AB07204C}" name="Tableau4" displayName="Tableau4" ref="A1:D7" totalsRowShown="0">
-  <autoFilter ref="A1:D7" xr:uid="{83DE1AE3-FEA1-4540-8E88-7AF1AB07204C}"/>
-  <tableColumns count="4">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{83DE1AE3-FEA1-4540-8E88-7AF1AB07204C}" name="Tableau4" displayName="Tableau4" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{83DE1AE3-FEA1-4540-8E88-7AF1AB07204C}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{20A36378-5423-4E16-8302-A28A97794E34}" name="user_id"/>
     <tableColumn id="2" xr3:uid="{36FAA869-4CAB-4E30-855B-9E0D61470286}" name="user_name"/>
     <tableColumn id="3" xr3:uid="{7B7CA9A5-917F-44D1-A329-7728A39CBB3D}" name="age"/>
     <tableColumn id="4" xr3:uid="{BD58BC77-FF3F-41FC-9A78-7BA9BB1377D6}" name="department"/>
+    <tableColumn id="5" xr3:uid="{B507704F-9BBF-4AE8-A8F0-374A6465395D}" name="car_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -598,7 +936,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,16 +949,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1910</v>
@@ -642,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1899</v>
@@ -656,7 +994,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1903</v>
@@ -676,10 +1014,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A87AAB8-04DF-4324-909A-166EE9FDB352}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,148 +1025,110 @@
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>147</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>37169</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>154200</v>
       </c>
-      <c r="F2">
+      <c r="E2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44084</v>
+      </c>
+      <c r="D3">
+        <v>27044</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>32880</v>
+      </c>
+      <c r="D4">
+        <v>184725</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41693</v>
+      </c>
+      <c r="D5">
+        <v>54227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C6" s="1">
         <v>44084</v>
       </c>
-      <c r="E3">
-        <v>27044</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>32880</v>
-      </c>
-      <c r="E4">
-        <v>184725</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>500</v>
-      </c>
-      <c r="D5" s="1">
-        <v>41693</v>
-      </c>
-      <c r="E5">
-        <v>54227</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44084</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
         <v>89721</v>
       </c>
-      <c r="F6">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="1">
         <v>44085</v>
       </c>
-      <c r="E7">
+      <c r="D7">
         <v>125416</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -840,12 +1140,111 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3346736-F25C-4565-9CD2-2A3B318F0AD0}">
+  <sheetPr codeName="Feuil5"/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1439D7-523E-49A7-BC6F-D94AB967805B}">
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,10 +1254,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,7 +1273,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -885,13 +1284,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F8F484-043C-45A2-AE8B-DE577714D350}">
   <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,102 +1299,123 @@
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1006,17 +1426,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CA4B13-7506-4CB3-A116-EFB484250679}">
-  <sheetPr codeName="Feuil18"/>
-  <dimension ref="A1:E17"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416D338E-A024-4BC1-BCDA-BB1AC694B97E}">
+  <sheetPr codeName="Feuil9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -1024,147 +1446,199 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
+      <c r="E19" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>